<commit_message>
added render functions to table
</commit_message>
<xml_diff>
--- a/Resource Analysis UI Mockup.xlsx
+++ b/Resource Analysis UI Mockup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpire\Code\Resource Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C7F6C-921F-4D5D-9BC4-A093770DC5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9802DE3D-BCAC-4EF9-8E02-C890A8974C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED383841-D49B-4BD7-8CA2-1B755375DC49}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,39 +459,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -843,7 +842,7 @@
   <dimension ref="C1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,10 +854,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="24"/>
+      <c r="K1" s="25"/>
       <c r="N1" t="s">
         <v>24</v>
       </c>
@@ -943,34 +942,33 @@
     </row>
     <row r="7" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="21" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="21" t="s">
+      <c r="G7" s="27"/>
+      <c r="H7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="27" t="s">
+      <c r="I7" s="27"/>
+      <c r="L7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="28"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="27" t="s">
+      <c r="M7" s="29"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="33" t="s">
+      <c r="P7" s="29"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="S7" s="21"/>
-      <c r="T7" s="22"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="27"/>
       <c r="W7" t="s">
         <v>30</v>
       </c>
@@ -995,17 +993,16 @@
       <c r="I8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="M8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N8" s="31" t="s">
+      <c r="N8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="30" t="s">
+      <c r="O8" s="22" t="s">
         <v>18</v>
       </c>
       <c r="P8" s="15" t="s">
@@ -1014,7 +1011,7 @@
       <c r="Q8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="R8" s="30" t="s">
+      <c r="R8" s="22" t="s">
         <v>18</v>
       </c>
       <c r="S8" s="15" t="s">
@@ -1062,19 +1059,19 @@
         <f>SUBTOTAL(9,L10:L21)</f>
         <v>5</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="24">
         <f>SUBTOTAL(9,M10:M21)</f>
         <v>3.5416666666666665</v>
       </c>
       <c r="N9" s="9">
-        <f t="shared" ref="N9:T9" si="1">SUBTOTAL(9,N10:N21)</f>
+        <f t="shared" ref="N9:Q9" si="1">SUBTOTAL(9,N10:N21)</f>
         <v>2.9166666666666665</v>
       </c>
       <c r="O9" s="8">
         <f>SUBTOTAL(9,O10:O21)</f>
         <v>5</v>
       </c>
-      <c r="P9" s="32">
+      <c r="P9" s="24">
         <f t="shared" si="1"/>
         <v>3.5416666666666665</v>
       </c>
@@ -1086,7 +1083,7 @@
         <f t="shared" ref="R9" si="2">L9+O9</f>
         <v>10</v>
       </c>
-      <c r="S9" s="32">
+      <c r="S9" s="24">
         <f>M9+P9</f>
         <v>7.083333333333333</v>
       </c>
@@ -1379,7 +1376,7 @@
       <c r="L14" s="8">
         <v>1.6666666666666667</v>
       </c>
-      <c r="M14" s="32">
+      <c r="M14" s="24">
         <f>SUBTOTAL(9,M15:M18)</f>
         <v>1.0416666666666665</v>
       </c>
@@ -1798,15 +1795,15 @@
     </row>
     <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="27"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="23" t="s">
+      <c r="L24" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="22"/>
+      <c r="M24" s="27"/>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
@@ -2106,6 +2103,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="R7:T7"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="L7:N7"/>
@@ -2113,8 +2112,6 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="L24:M24"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="R7:T7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{AF915600-9F3C-43B7-B825-E825034E34D4}">

</xml_diff>